<commit_message>
i cannot find the exact modification in code
</commit_message>
<xml_diff>
--- a/searchbar/search_items.xlsx
+++ b/searchbar/search_items.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">items</t>
   </si>
@@ -41,6 +41,15 @@
   </si>
   <si>
     <t xml:space="preserve">airpods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">graphic card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bike chain cleaner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bike chain lube</t>
   </si>
 </sst>
 </file>
@@ -317,10 +326,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1048576"/>
+  <dimension ref="A1:A1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -331,34 +340,29 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -368,6 +372,21 @@
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>